<commit_message>
Improved heightmap convertion formula
</commit_message>
<xml_diff>
--- a/project/LinearReg.xlsx
+++ b/project/LinearReg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrofonseca/Documents/FEUP/CG/cg-t02-g05/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBFB3B2B-3735-C741-B256-756B7415E1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80DE5F8-66EA-D347-96CF-AB959836F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{20E33619-CB1C-7347-AFFA-15851449185E}"/>
+    <workbookView xWindow="-900" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{20E33619-CB1C-7347-AFFA-15851449185E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,7 +170,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -206,10 +207,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$7</c:f>
+              <c:f>Sheet1!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>110</c:v>
                 </c:pt>
@@ -219,15 +220,18 @@
                 <c:pt idx="2">
                   <c:v>157</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>237</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$7</c:f>
+              <c:f>Sheet1!$A$5:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>-60</c:v>
                 </c:pt>
@@ -236,6 +240,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>-48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1321,9 +1328,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C302D17C-B66E-7B4A-AD20-2216892C1066}">
-  <dimension ref="A5:B7"/>
+  <dimension ref="A5:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="169" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="169" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1353,6 +1360,14 @@
         <v>157</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>-27</v>
+      </c>
+      <c r="B8">
+        <v>237</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>